<commit_message>
add file length checking in CustomDatasest (dataloader.py), improved breakpoint function generation, added ability to have any number of parameters with any name (at the column head of the excel file)
</commit_message>
<xml_diff>
--- a/testdata/dac-train.xlsx
+++ b/testdata/dac-train.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2024_dacSynthformer\DACSynthformer\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2025_Synthformer\DACSynthformer\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F65C40-57E4-4C92-9B7F-D025FAD546AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120ED13A-FE28-41BE-91F5-D5AC1451E3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5963" yWindow="4673" windowWidth="22500" windowHeight="13912" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1087" windowWidth="22500" windowHeight="13913" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,6 @@
     <t>Param1</t>
   </si>
   <si>
-    <t>Param2</t>
-  </si>
-  <si>
-    <t>Param3</t>
-  </si>
-  <si>
     <t>DSBugs</t>
   </si>
   <si>
@@ -59,6 +53,12 @@
   </si>
   <si>
     <t>DSWind--strength-00.50--c-00--x-90.dac</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>bar</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D1" sqref="D1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -443,78 +443,78 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="E2">
-        <v>72</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="E3">
-        <v>90</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="E4">
-        <v>66</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="E5">
-        <v>88</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>